<commit_message>
added methods to collect important epidemiological indicators
</commit_message>
<xml_diff>
--- a/rate_matrix.xlsx
+++ b/rate_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vijetadeshpande/Documents/GitHub/compartmental-model-COVID19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCA74B4-70AF-6F4D-ACF0-321D317064E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F559DF0-A235-134E-9FFE-22E8D5A217D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{68BC5988-E0E2-3145-9802-2A71AB6DCC1D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{68BC5988-E0E2-3145-9802-2A71AB6DCC1D}"/>
   </bookViews>
   <sheets>
     <sheet name="rate matrix" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -509,11 +509,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{469C106C-C0BF-6E4A-8EFB-4C5B408BEA35}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
@@ -521,7 +521,7 @@
     <col min="11" max="12" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -544,7 +544,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -565,7 +565,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -587,7 +587,7 @@
       <c r="I3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -608,7 +608,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -630,7 +630,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -652,7 +652,7 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -671,15 +671,15 @@
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I8" s="1"/>
     </row>
@@ -692,11 +692,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8DE0EB-6EE2-C94D-98D4-90D7B73D6803}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
@@ -704,7 +704,7 @@
     <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -727,7 +727,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -747,7 +747,7 @@
         <v>4.0070781027607166E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -767,7 +767,7 @@
         <v>2.3839999999999998E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -787,7 +787,7 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -808,7 +808,7 @@
         <v>4.0070781027607166E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -829,7 +829,7 @@
         <v>5.128205128205128E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -847,20 +847,18 @@
         <v>4.0070781027607166E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="9">
-        <v>1</v>
-      </c>
+      <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -876,13 +874,13 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:9">
       <c r="B2" t="s">
         <v>16</v>
       </c>
@@ -899,7 +897,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9">
       <c r="B3" t="s">
         <v>21</v>
       </c>
@@ -920,7 +918,7 @@
         <v>2.3845999999999993E-3</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" ht="18">
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
@@ -945,7 +943,7 @@
         <v>1.8000000000000002E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9" ht="18">
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
@@ -970,7 +968,7 @@
         <v>1.8000000000000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9" ht="18">
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
@@ -995,7 +993,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9" ht="18">
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1020,7 +1018,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:9" ht="18">
       <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1045,7 +1043,7 @@
         <v>5.7999999999999996E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:9" ht="18">
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1070,7 +1068,7 @@
         <v>5.7999999999999996E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:9" ht="18">
       <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1095,7 +1093,7 @@
         <v>5.7999999999999996E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:9" ht="18">
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1120,7 +1118,7 @@
         <v>5.7999999999999996E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:9" ht="18">
       <c r="B12" s="2" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
started writing structure for optimization module required for parameterization
</commit_message>
<xml_diff>
--- a/rate_matrix.xlsx
+++ b/rate_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vijetadeshpande/Documents/GitHub/compartmental-model-COVID19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F559DF0-A235-134E-9FFE-22E8D5A217D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B505E07-9783-E647-BA22-328B89F1DF1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{68BC5988-E0E2-3145-9802-2A71AB6DCC1D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>Exposed</t>
   </si>
@@ -101,14 +101,39 @@
   </si>
   <si>
     <t>&lt;60</t>
+  </si>
+  <si>
+    <t>exposed</t>
+  </si>
+  <si>
+    <t>symptomatic</t>
+  </si>
+  <si>
+    <t>diagnosed</t>
+  </si>
+  <si>
+    <t>non-severe cases</t>
+  </si>
+  <si>
+    <t>severe cases</t>
+  </si>
+  <si>
+    <t>recovery</t>
+  </si>
+  <si>
+    <t>death</t>
+  </si>
+  <si>
+    <t>births</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -125,18 +150,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -181,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -190,9 +209,12 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{469C106C-C0BF-6E4A-8EFB-4C5B408BEA35}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -523,165 +545,188 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <f>-SUM(C2:H2)</f>
-        <v>-9.0949161690118518E-2</v>
-      </c>
-      <c r="C2" s="1">
-        <v>9.0909090909090912E-2</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1">
-        <f>1/(68.56*52*7)</f>
-        <v>4.0070781027607166E-5</v>
-      </c>
-      <c r="I2" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="B2">
+        <v>-1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="11"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>1.2</v>
+      </c>
       <c r="C3" s="1">
-        <f>-SUM(D3:H3)</f>
-        <v>-1</v>
-      </c>
-      <c r="D3" s="4">
-        <f>1-H3</f>
-        <v>0.99761599999999995</v>
+        <f>-SUM(D3:I3)</f>
+        <v>-9.0949196788612852E-2</v>
+      </c>
+      <c r="D3" s="1">
+        <f>1/11</f>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="1">
-        <v>2.3839999999999998E-3</v>
-      </c>
-      <c r="I3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1">
+        <f>I8</f>
+        <v>4.0105879521937915E-5</v>
+      </c>
+      <c r="J3" s="11"/>
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>1.2</v>
+      </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="4">
-        <f>-SUM(E4:F4)</f>
+      <c r="D4" s="1">
+        <f>-SUM(E4:I4)</f>
         <v>-1</v>
       </c>
-      <c r="E4" s="4">
-        <f>1-F4</f>
-        <v>0.83</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.17</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="E4" s="10">
+        <f>1-SUM(F4:I4)</f>
+        <v>0.94264323997170707</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10">
+        <f>0.8*(1/14)</f>
+        <v>5.7142857142857141E-2</v>
+      </c>
+      <c r="I4" s="10">
+        <f>(0.8*I8)+(0.2*0.02*1/22)</f>
+        <v>2.1390288543573217E-4</v>
+      </c>
+      <c r="J4" s="11"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1"/>
+        <v>24</v>
+      </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1">
-        <f>-SUM(G5:H5)</f>
-        <v>-0.10004007078102761</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="4">
-        <f>1/10</f>
-        <v>0.1</v>
-      </c>
-      <c r="H5" s="4">
-        <f>H7</f>
-        <v>4.0070781027607166E-5</v>
-      </c>
-      <c r="I5" s="1"/>
+      <c r="E5" s="10">
+        <f>-SUM(F5:H5)</f>
+        <v>-0.10571428571428571</v>
+      </c>
+      <c r="F5" s="10">
+        <f xml:space="preserve"> 0.2*(1/7)</f>
+        <v>2.8571428571428571E-2</v>
+      </c>
+      <c r="G5" s="10">
+        <f>0.2*1/10</f>
+        <v>0.02</v>
+      </c>
+      <c r="H5" s="10">
+        <f>0.8*(1/14)</f>
+        <v>5.7142857142857141E-2</v>
+      </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="11"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1"/>
+        <v>25</v>
+      </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1">
-        <f>-SUM(G6:H6)</f>
-        <v>-9.6736596736596736E-2</v>
-      </c>
-      <c r="G6" s="1">
-        <f>1/22</f>
-        <v>4.5454545454545456E-2</v>
-      </c>
-      <c r="H6" s="1">
-        <f>1/19.5</f>
-        <v>5.128205128205128E-2</v>
-      </c>
-      <c r="I6" s="1"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10">
+        <f>-SUM(H6:I6)</f>
+        <v>-9.4073377234242708E-2</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10">
+        <f>1/10.63</f>
+        <v>9.4073377234242708E-2</v>
+      </c>
+      <c r="I6" s="10"/>
+      <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1"/>
+        <v>26</v>
+      </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1">
-        <f>-H7</f>
-        <v>-4.0070781027607166E-5</v>
+        <f>-SUM(H7:I7)</f>
+        <v>-9.6736596736596736E-2</v>
       </c>
       <c r="H7" s="1">
-        <f>H2</f>
-        <v>4.0070781027607166E-5</v>
-      </c>
-      <c r="I7" s="1"/>
+        <f>1/22</f>
+        <v>4.5454545454545456E-2</v>
+      </c>
+      <c r="I7" s="1">
+        <f>1/19.5</f>
+        <v>5.128205128205128E-2</v>
+      </c>
+      <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1">
+        <f>-I8</f>
+        <v>-4.0105879521937915E-5</v>
+      </c>
+      <c r="I8" s="1">
+        <f>1/(68.5*52*7)</f>
+        <v>4.0105879521937915E-5</v>
+      </c>
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9">
         <v>0</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -731,18 +776,18 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <f>-SUM(C2:H2)</f>
         <v>-9.0949161690118518E-2</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="7">
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="6">
         <f>1/(68.56*52*7)</f>
         <v>4.0070781027607166E-5</v>
       </c>
@@ -751,19 +796,19 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5">
         <f>-SUM(D3:H3)</f>
         <v>-1</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <f>1-H3</f>
         <v>0.99761599999999995</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="7">
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="6">
         <v>2.3839999999999998E-3</v>
       </c>
     </row>
@@ -771,39 +816,39 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5">
         <f>-SUM(E4:F4)</f>
         <v>-1</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <f>1-F4</f>
         <v>0.83</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="9">
         <v>0.17</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5">
         <f>-SUM(G5:H5)</f>
         <v>-0.10004007078102761</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="8">
+      <c r="F5" s="5"/>
+      <c r="G5" s="7">
         <f>1/10</f>
         <v>0.1</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="7">
         <f>H7</f>
         <v>4.0070781027607166E-5</v>
       </c>
@@ -812,19 +857,19 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5">
         <f>-SUM(G6:H6)</f>
         <v>-9.6736596736596736E-2</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <f>1/22</f>
         <v>4.5454545454545456E-2</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <f>1/19.5</f>
         <v>5.128205128205128E-2</v>
       </c>
@@ -833,16 +878,16 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5">
         <f>-H7</f>
         <v>-4.0070781027607166E-5</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <f>H2</f>
         <v>4.0070781027607166E-5</v>
       </c>
@@ -851,13 +896,13 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made few chnages in the calibration model
</commit_message>
<xml_diff>
--- a/rate_matrix.xlsx
+++ b/rate_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vijetadeshpande/Documents/GitHub/compartmental-model-COVID19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B505E07-9783-E647-BA22-328B89F1DF1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712903C8-E2EF-724F-AEFA-1095CA41623E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{68BC5988-E0E2-3145-9802-2A71AB6DCC1D}"/>
   </bookViews>
@@ -532,7 +532,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
added another compartment to differentiate between exposed and asymptomatic
</commit_message>
<xml_diff>
--- a/rate_matrix.xlsx
+++ b/rate_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vijetadeshpande/Documents/GitHub/compartmental-model-COVID19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB2A9E2-8BE3-1047-8F84-337E2F3CFC61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CE9C0B-2693-7C47-AC0A-62E7C2EDF951}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{68BC5988-E0E2-3145-9802-2A71AB6DCC1D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>Exposed</t>
   </si>
@@ -125,15 +125,17 @@
   </si>
   <si>
     <t>births</t>
+  </si>
+  <si>
+    <t>asymptomatic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
-    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -200,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -212,9 +214,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{469C106C-C0BF-6E4A-8EFB-4C5B408BEA35}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -543,7 +542,7 @@
     <col min="11" max="12" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:10">
       <c r="B1" t="s">
         <v>29</v>
       </c>
@@ -551,25 +550,28 @@
         <v>22</v>
       </c>
       <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -579,152 +581,162 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="J2" s="11"/>
-    </row>
-    <row r="3" spans="1:12">
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>22</v>
       </c>
-      <c r="B3">
-        <v>1.2</v>
-      </c>
       <c r="C3" s="1">
-        <f>-SUM(D3:I3)</f>
-        <v>-9.0949196788612852E-2</v>
-      </c>
-      <c r="D3" s="1">
-        <f>1/11</f>
-        <v>9.0909090909090912E-2</v>
+        <f>-SUM(D3:J3)</f>
+        <v>-0.11786096170896514</v>
+      </c>
+      <c r="D3">
+        <f>1/8.5</f>
+        <v>0.11764705882352941</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="1">
-        <f>I8</f>
-        <v>4.0105879521937915E-5</v>
-      </c>
-      <c r="J3" s="11"/>
-      <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="I3" s="1"/>
+      <c r="J3" s="10">
+        <f>(0.8*(1/(68.5*52*7)))+(0.2*0.02*1/22)</f>
+        <v>2.1390288543573217E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>1.2</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1">
-        <f>-SUM(E4:I4)</f>
+      <c r="D4">
+        <f>-SUM(E4:J4)</f>
+        <v>-0.40021390288543573</v>
+      </c>
+      <c r="E4">
+        <f>1/2.5</f>
+        <v>0.4</v>
+      </c>
+      <c r="J4" s="10">
+        <f>(0.8*(1/(68.5*52*7)))+(0.2*0.02*1/22)</f>
+        <v>2.1390288543573217E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>1.2</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="E5" s="1">
+        <f>-SUM(F5:J5)</f>
         <v>-1</v>
       </c>
-      <c r="E4" s="10">
-        <f>1-SUM(F4:I4)</f>
+      <c r="F5" s="10">
+        <f>1-SUM(G5:J5)</f>
         <v>0.94264323997170707</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10">
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10">
         <f>0.8*(1/14)</f>
         <v>5.7142857142857141E-2</v>
       </c>
-      <c r="I4" s="10">
-        <f>(0.8*I8)+(0.2*0.02*1/22)</f>
+      <c r="J5" s="10">
+        <f>(0.8*(1/(68.5*52*7)))+(0.2*0.02*1/22)</f>
         <v>2.1390288543573217E-4</v>
       </c>
-      <c r="J4" s="11"/>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s">
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="10">
-        <f>-SUM(F5:H5)</f>
+      <c r="C6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="10">
+        <f>-SUM(G6:I6)</f>
         <v>-0.10571428571428571</v>
       </c>
-      <c r="F5" s="10">
+      <c r="G6" s="10">
         <f xml:space="preserve"> 0.2*(1/7)</f>
         <v>2.8571428571428571E-2</v>
       </c>
-      <c r="G5" s="10">
+      <c r="H6" s="10">
         <f>0.2*1/10</f>
         <v>0.02</v>
       </c>
-      <c r="H5" s="10">
+      <c r="I6" s="10">
         <f>0.8*(1/14)</f>
         <v>5.7142857142857141E-2</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="11"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" t="s">
+      <c r="J6" s="10"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10">
-        <f>-SUM(H6:I6)</f>
+      <c r="C7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10">
+        <f>-SUM(I7:J7)</f>
         <v>-9.4073377234242708E-2</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10">
+      <c r="H7" s="10"/>
+      <c r="I7" s="10">
         <f>1/10.63</f>
         <v>9.4073377234242708E-2</v>
       </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="11"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" t="s">
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1">
-        <f>-SUM(H7:I7)</f>
-        <v>-9.6736596736596736E-2</v>
-      </c>
-      <c r="H7" s="1">
-        <f>1/22</f>
-        <v>4.5454545454545456E-2</v>
-      </c>
-      <c r="I7" s="1">
-        <f>1/19.5</f>
-        <v>5.128205128205128E-2</v>
-      </c>
-      <c r="J7" s="11"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1">
-        <f>-I8</f>
+        <f>-SUM(I8:J8)</f>
+        <v>-9.6736596736596736E-2</v>
+      </c>
+      <c r="I8" s="1">
+        <f>1/22</f>
+        <v>4.5454545454545456E-2</v>
+      </c>
+      <c r="J8" s="1">
+        <f>1/19.5</f>
+        <v>5.128205128205128E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1">
+        <f>-J9</f>
         <v>-4.0105879521937915E-5</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J9" s="1">
         <f>1/(68.5*52*7)</f>
         <v>4.0105879521937915E-5</v>
       </c>
-      <c r="J8" s="11"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" t="s">
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
         <v>28</v>
       </c>
-      <c r="I9">
+      <c r="J10">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added data processing code to create df having different data features which can be used to calibrate model
</commit_message>
<xml_diff>
--- a/rate_matrix.xlsx
+++ b/rate_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vijetadeshpande/Documents/GitHub/compartmental-model-COVID19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CE9C0B-2693-7C47-AC0A-62E7C2EDF951}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D0812D-C5E0-CC4E-B484-07847719AFA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{68BC5988-E0E2-3145-9802-2A71AB6DCC1D}"/>
   </bookViews>
@@ -531,7 +531,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -609,7 +609,8 @@
         <v>30</v>
       </c>
       <c r="B4">
-        <v>1.2</v>
+        <f>(2.2/(11-2.5))</f>
+        <v>0.25882352941176473</v>
       </c>
       <c r="D4">
         <f>-SUM(E4:J4)</f>
@@ -629,7 +630,8 @@
         <v>23</v>
       </c>
       <c r="B5">
-        <v>1.2</v>
+        <f>(2.2/(11-2.5))</f>
+        <v>0.25882352941176473</v>
       </c>
       <c r="C5" s="1"/>
       <c r="E5" s="1">

</xml_diff>